<commit_message>
temp fixes for bus issue
</commit_message>
<xml_diff>
--- a/InputData/trans/BRZSPbS/BAU Required ZEV Sales Perc by Subregion.xlsx
+++ b/InputData/trans/BRZSPbS/BAU Required ZEV Sales Perc by Subregion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\trans\BRZSPbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD3259B-B54A-41F8-8532-9ED733F4E0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F19244-1E35-42A6-81E2-A01BB1F79441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60285" yWindow="3225" windowWidth="21600" windowHeight="12525" firstSheet="2" activeTab="5" xr2:uid="{8F1AFB95-7E48-4A2A-86D9-67ED7638AFF8}"/>
+    <workbookView xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="12525" activeTab="2" xr2:uid="{8F1AFB95-7E48-4A2A-86D9-67ED7638AFF8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -942,15 +942,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE72620-2405-41A9-A74D-2CDDCE0D4B8D}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="73.453125" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1021,80 +1022,93 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
         <v>2022</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>5000</v>
+      </c>
+      <c r="I17">
+        <f>H17*(1-(1+H18)^-H19)/H18</f>
+        <v>34919.196990561657</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" s="4">
         <v>2021</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1144,6 +1158,9 @@
       <c r="A54" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1" xr:uid="{E5467C05-C70C-4E5C-ADAD-9E68FF892FF9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1155,8 +1172,8 @@
   </sheetPr>
   <dimension ref="A1:AF61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AF28"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7154,8 +7171,8 @@
   </sheetPr>
   <dimension ref="A1:AF61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AF28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7284,79 +7301,104 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.3</v>
+        <f>0.301*0.46</f>
+        <v>0.13846</v>
       </c>
       <c r="I2">
-        <v>0.3</v>
+        <f>H2</f>
+        <v>0.13846</v>
       </c>
       <c r="J2">
-        <v>0.3</v>
+        <f t="shared" ref="J2:AF2" si="0">I2</f>
+        <v>0.13846</v>
       </c>
       <c r="K2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="L2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="M2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="N2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="O2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="P2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="Q2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="R2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="S2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="T2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="U2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="V2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="W2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="X2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="Y2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="Z2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="AA2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="AB2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="AC2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="AD2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="AE2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
       <c r="AF2">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
@@ -7382,79 +7424,104 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.3</v>
+        <f t="shared" ref="H3:H28" si="1">0.301*0.46</f>
+        <v>0.13846</v>
       </c>
       <c r="I3">
-        <v>0.3</v>
+        <f t="shared" ref="I3:AF3" si="2">H3</f>
+        <v>0.13846</v>
       </c>
       <c r="J3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="K3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="L3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="M3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="N3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="O3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="P3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="Q3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="R3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="S3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="T3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="U3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="V3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="W3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="X3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="Y3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="Z3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="AA3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="AB3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="AC3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="AD3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="AE3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
       <c r="AF3">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
@@ -7480,79 +7547,104 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I4">
-        <v>0.3</v>
+        <f t="shared" ref="I4:AF4" si="3">H4</f>
+        <v>0.13846</v>
       </c>
       <c r="J4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="K4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="L4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="M4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="N4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="O4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="P4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="Q4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="R4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="S4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="T4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="U4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="V4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="W4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="X4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="Y4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="Z4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="AA4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="AB4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="AC4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="AD4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="AE4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
       <c r="AF4">
-        <v>0.3</v>
+        <f t="shared" si="3"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
@@ -7578,79 +7670,104 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I5">
-        <v>0.3</v>
+        <f t="shared" ref="I5:AF5" si="4">H5</f>
+        <v>0.13846</v>
       </c>
       <c r="J5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="K5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="L5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="M5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="N5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="O5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="P5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="Q5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="R5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="S5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="T5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="U5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="V5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="W5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="X5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="Y5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="Z5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="AA5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="AB5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="AC5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="AD5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="AE5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
       <c r="AF5">
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
@@ -7676,79 +7793,104 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I6">
-        <v>0.3</v>
+        <f t="shared" ref="I6:AF6" si="5">H6</f>
+        <v>0.13846</v>
       </c>
       <c r="J6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="K6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="L6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="M6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="N6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="O6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="P6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="Q6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="R6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="S6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="T6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="U6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="V6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="W6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="X6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="Y6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="Z6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="AA6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="AB6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="AC6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="AD6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="AE6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
       <c r="AF6">
-        <v>0.3</v>
+        <f t="shared" si="5"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -7774,79 +7916,104 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I7">
-        <v>0.3</v>
+        <f t="shared" ref="I7:AF7" si="6">H7</f>
+        <v>0.13846</v>
       </c>
       <c r="J7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="K7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="L7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="M7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="N7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="O7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="P7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="Q7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="R7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="S7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="T7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="U7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="V7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="W7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="X7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="Y7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="Z7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="AA7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="AB7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="AC7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="AD7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="AE7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
       <c r="AF7">
-        <v>0.3</v>
+        <f t="shared" si="6"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.35">
@@ -7872,79 +8039,104 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I8">
-        <v>0.3</v>
+        <f t="shared" ref="I8:AF8" si="7">H8</f>
+        <v>0.13846</v>
       </c>
       <c r="J8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="K8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="L8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="M8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="N8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="O8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="P8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="Q8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="R8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="S8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="T8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="U8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="V8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="W8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="X8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="Y8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="Z8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="AA8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="AB8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="AC8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="AD8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="AE8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
       <c r="AF8">
-        <v>0.3</v>
+        <f t="shared" si="7"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.35">
@@ -7970,79 +8162,104 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I9">
-        <v>0.3</v>
+        <f t="shared" ref="I9:AF9" si="8">H9</f>
+        <v>0.13846</v>
       </c>
       <c r="J9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="K9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="L9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="M9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="N9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="O9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="P9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="Q9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="R9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="S9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="T9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="U9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="V9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="W9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="X9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="Y9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="Z9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="AA9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="AB9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="AC9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="AD9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="AE9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
       <c r="AF9">
-        <v>0.3</v>
+        <f t="shared" si="8"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.35">
@@ -8068,79 +8285,104 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I10">
-        <v>0.3</v>
+        <f t="shared" ref="I10:AF10" si="9">H10</f>
+        <v>0.13846</v>
       </c>
       <c r="J10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="K10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="L10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="M10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="N10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="O10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="P10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="Q10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="R10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="S10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="T10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="U10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="V10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="W10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="X10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="Y10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="Z10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="AA10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="AB10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="AC10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="AD10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="AE10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
       <c r="AF10">
-        <v>0.3</v>
+        <f t="shared" si="9"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.35">
@@ -8166,79 +8408,104 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I11">
-        <v>0.3</v>
+        <f t="shared" ref="I11:AF11" si="10">H11</f>
+        <v>0.13846</v>
       </c>
       <c r="J11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="K11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="L11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="M11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="N11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="O11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="P11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="Q11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="R11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="S11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="T11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="U11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="V11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="W11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="X11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="Y11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="Z11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="AA11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="AB11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="AC11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="AD11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="AE11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
       <c r="AF11">
-        <v>0.3</v>
+        <f t="shared" si="10"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
@@ -8264,79 +8531,104 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I12">
-        <v>0.3</v>
+        <f t="shared" ref="I12:AF12" si="11">H12</f>
+        <v>0.13846</v>
       </c>
       <c r="J12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="K12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="L12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="M12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="N12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="O12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="P12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="Q12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="R12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="S12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="T12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="U12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="V12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="W12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="X12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="Y12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="Z12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="AA12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="AB12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="AC12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="AD12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="AE12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
       <c r="AF12">
-        <v>0.3</v>
+        <f t="shared" si="11"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.35">
@@ -8362,79 +8654,104 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I13">
-        <v>0.3</v>
+        <f t="shared" ref="I13:AF13" si="12">H13</f>
+        <v>0.13846</v>
       </c>
       <c r="J13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="K13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="L13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="M13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="N13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="O13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="P13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="Q13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="R13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="S13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="T13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="U13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="V13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="W13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="X13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="Y13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="Z13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="AA13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="AB13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="AC13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="AD13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="AE13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
       <c r="AF13">
-        <v>0.3</v>
+        <f t="shared" si="12"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.35">
@@ -8460,79 +8777,104 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I14">
-        <v>0.3</v>
+        <f t="shared" ref="I14:AF14" si="13">H14</f>
+        <v>0.13846</v>
       </c>
       <c r="J14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="K14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="L14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="M14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="N14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="O14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="P14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="Q14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="R14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="S14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="T14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="U14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="V14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="W14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="X14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="Y14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="Z14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="AA14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="AB14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="AC14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="AD14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="AE14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
       <c r="AF14">
-        <v>0.3</v>
+        <f t="shared" si="13"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.35">
@@ -8558,79 +8900,104 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I15">
-        <v>0.3</v>
+        <f t="shared" ref="I15:AF15" si="14">H15</f>
+        <v>0.13846</v>
       </c>
       <c r="J15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="K15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="L15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="M15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="N15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="O15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="P15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="Q15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="R15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="S15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="T15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="U15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="V15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="W15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="X15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="Y15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="Z15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="AA15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="AB15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="AC15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="AD15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="AE15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
       <c r="AF15">
-        <v>0.3</v>
+        <f t="shared" si="14"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.35">
@@ -8656,79 +9023,104 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I16">
-        <v>0.3</v>
+        <f t="shared" ref="I16:AF16" si="15">H16</f>
+        <v>0.13846</v>
       </c>
       <c r="J16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="K16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="L16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="M16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="N16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="O16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="P16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="Q16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="R16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="S16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="T16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="U16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="V16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="W16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="X16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="Y16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="Z16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="AA16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="AB16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="AC16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="AD16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="AE16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
       <c r="AF16">
-        <v>0.3</v>
+        <f t="shared" si="15"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.35">
@@ -8754,79 +9146,104 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I17">
-        <v>0.3</v>
+        <f t="shared" ref="I17:AF17" si="16">H17</f>
+        <v>0.13846</v>
       </c>
       <c r="J17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="K17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="L17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="M17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="N17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="O17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="P17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="Q17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="R17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="S17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="T17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="U17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="V17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="W17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="X17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="Y17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="Z17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="AA17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="AB17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="AC17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="AD17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="AE17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
       <c r="AF17">
-        <v>0.3</v>
+        <f t="shared" si="16"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.35">
@@ -8852,79 +9269,104 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I18">
-        <v>0.3</v>
+        <f t="shared" ref="I18:AF18" si="17">H18</f>
+        <v>0.13846</v>
       </c>
       <c r="J18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="K18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="L18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="M18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="N18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="O18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="P18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="Q18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="R18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="S18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="T18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="U18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="V18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="W18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="X18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="Y18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="Z18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="AA18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="AB18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="AC18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="AD18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="AE18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
       <c r="AF18">
-        <v>0.3</v>
+        <f t="shared" si="17"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.35">
@@ -8950,79 +9392,104 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I19">
-        <v>0.3</v>
+        <f t="shared" ref="I19:AF19" si="18">H19</f>
+        <v>0.13846</v>
       </c>
       <c r="J19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="K19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="L19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="M19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="N19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="O19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="P19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="Q19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="R19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="S19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="T19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="U19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="V19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="W19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="X19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="Y19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="Z19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="AA19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="AB19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="AC19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="AD19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="AE19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
       <c r="AF19">
-        <v>0.3</v>
+        <f t="shared" si="18"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.35">
@@ -9048,79 +9515,104 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I20">
-        <v>0.3</v>
+        <f t="shared" ref="I20:AF20" si="19">H20</f>
+        <v>0.13846</v>
       </c>
       <c r="J20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="K20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="L20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="M20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="N20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="O20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="P20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="Q20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="R20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="S20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="T20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="U20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="V20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="W20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="X20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="Y20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="Z20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="AA20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="AB20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="AC20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="AD20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="AE20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
       <c r="AF20">
-        <v>0.3</v>
+        <f t="shared" si="19"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.35">
@@ -9146,79 +9638,104 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I21">
-        <v>0.3</v>
+        <f t="shared" ref="I21:AF21" si="20">H21</f>
+        <v>0.13846</v>
       </c>
       <c r="J21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="K21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="L21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="M21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="N21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="O21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="P21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="Q21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="R21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="S21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="T21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="U21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="V21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="W21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="X21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="Y21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="Z21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="AA21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="AB21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="AC21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="AD21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="AE21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
       <c r="AF21">
-        <v>0.3</v>
+        <f t="shared" si="20"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.35">
@@ -9244,79 +9761,104 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I22">
-        <v>0.3</v>
+        <f t="shared" ref="I22:AF22" si="21">H22</f>
+        <v>0.13846</v>
       </c>
       <c r="J22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="K22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="L22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="M22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="N22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="O22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="P22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="Q22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="R22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="S22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="T22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="U22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="V22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="W22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="X22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="Y22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="Z22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="AA22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="AB22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="AC22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="AD22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="AE22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
       <c r="AF22">
-        <v>0.3</v>
+        <f t="shared" si="21"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.35">
@@ -9342,79 +9884,104 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I23">
-        <v>0.3</v>
+        <f t="shared" ref="I23:AF23" si="22">H23</f>
+        <v>0.13846</v>
       </c>
       <c r="J23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="K23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="L23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="M23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="N23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="O23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="P23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="Q23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="R23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="S23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="T23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="U23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="V23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="W23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="X23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="Y23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="Z23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="AA23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="AB23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="AC23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="AD23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="AE23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
       <c r="AF23">
-        <v>0.3</v>
+        <f t="shared" si="22"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.35">
@@ -9440,79 +10007,104 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I24">
-        <v>0.3</v>
+        <f t="shared" ref="I24:AF24" si="23">H24</f>
+        <v>0.13846</v>
       </c>
       <c r="J24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="K24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="L24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="M24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="N24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="O24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="P24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="Q24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="R24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="S24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="T24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="U24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="V24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="W24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="X24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="Y24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="Z24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="AA24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="AB24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="AC24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="AD24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="AE24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
       <c r="AF24">
-        <v>0.3</v>
+        <f t="shared" si="23"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.35">
@@ -9538,79 +10130,104 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I25">
-        <v>0.3</v>
+        <f t="shared" ref="I25:AF25" si="24">H25</f>
+        <v>0.13846</v>
       </c>
       <c r="J25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="K25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="L25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="M25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="N25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="O25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="P25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="Q25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="R25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="S25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="T25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="U25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="V25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="W25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="X25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="Y25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="Z25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="AA25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="AB25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="AC25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="AD25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="AE25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
       <c r="AF25">
-        <v>0.3</v>
+        <f t="shared" si="24"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.35">
@@ -9636,79 +10253,104 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I26">
-        <v>0.3</v>
+        <f t="shared" ref="I26:AF26" si="25">H26</f>
+        <v>0.13846</v>
       </c>
       <c r="J26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="K26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="L26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="M26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="N26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="O26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="P26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="Q26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="R26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="S26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="T26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="U26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="V26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="W26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="X26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="Y26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="Z26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="AA26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="AB26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="AC26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="AD26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="AE26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
       <c r="AF26">
-        <v>0.3</v>
+        <f t="shared" si="25"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.35">
@@ -9734,79 +10376,104 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I27">
-        <v>0.3</v>
+        <f t="shared" ref="I27:AF27" si="26">H27</f>
+        <v>0.13846</v>
       </c>
       <c r="J27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="K27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="L27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="M27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="N27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="O27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="P27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="Q27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="R27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="S27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="T27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="U27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="V27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="W27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="X27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="Y27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="Z27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="AA27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="AB27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="AC27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="AD27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="AE27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
       <c r="AF27">
-        <v>0.3</v>
+        <f t="shared" si="26"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.35">
@@ -9832,79 +10499,104 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.13846</v>
       </c>
       <c r="I28">
-        <v>0.3</v>
+        <f t="shared" ref="I28:AF28" si="27">H28</f>
+        <v>0.13846</v>
       </c>
       <c r="J28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="K28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="L28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="M28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="N28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="O28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="P28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="Q28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="R28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="S28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="T28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="U28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="V28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="W28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="X28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="Y28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="Z28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="AA28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="AB28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="AC28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="AD28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="AE28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
       <c r="AF28">
-        <v>0.3</v>
+        <f t="shared" si="27"/>
+        <v>0.13846</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.35">
@@ -25151,8 +25843,8 @@
   </sheetPr>
   <dimension ref="A1:AF61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AF28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -37143,26 +37835,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -37391,26 +38063,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C09B37-832A-4BED-856A-94AD65F214F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B62C4F-955D-4DE0-87FA-884D2F16A437}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2074C4B4-07F3-44D2-B5B3-B925F13ECF0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37427,4 +38100,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B62C4F-955D-4DE0-87FA-884D2F16A437}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C09B37-832A-4BED-856A-94AD65F214F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>